<commit_message>
Registered users' login (username and password verified). Template for 403 created (products/create for not authorised persons)
</commit_message>
<xml_diff>
--- a/NewsPaper/Questions_commands.xlsx
+++ b/NewsPaper/Questions_commands.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Natalija\PycharmProjects\Project_django_news\NewsPaper\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{EF7FC1B2-7FC4-4680-891E-AAF3B45C5CB3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2F34DA80-115B-434F-B7FD-E34DD51CE8D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{AC10997F-ADC5-405A-8327-3E730F94FD95}"/>
   </bookViews>
@@ -3838,8 +3838,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F30144BF-70AD-45CC-9A33-F55102E0E57A}">
   <dimension ref="A1:N105"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="H89" sqref="H89"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A65" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B95" sqref="B95"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>

</xml_diff>